<commit_message>
Added Nehwe Technologies LLC to devliverables
</commit_message>
<xml_diff>
--- a/CMMC-Demo-Aegis-Avionics/docs/02-assessment/Gap-Assessment.xlsx
+++ b/CMMC-Demo-Aegis-Avionics/docs/02-assessment/Gap-Assessment.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikael\Biz\NIST-800-171-Readiness-Assessment\CMMC-Demo-Aegis-Avionics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikael\Biz\NIST-800-171-Readiness-Assessment\CMMC-Demo-Aegis-Avionics\docs\02-assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8B459C-E590-460C-97E4-6E238CA7C1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC2F44B-0453-4B11-8812-5F9C49CE7487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{0AC88B97-F9F5-4B13-A825-936F26B68506}"/>
+    <workbookView xWindow="57480" yWindow="16170" windowWidth="29040" windowHeight="15720" xr2:uid="{0AC88B97-F9F5-4B13-A825-936F26B68506}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GAP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -744,22 +744,22 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="9.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.75" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.35546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15">
+    <row r="1" spans="1:7" ht="28.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -782,7 +782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="199.5">
+    <row r="2" spans="1:7" ht="198">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -805,7 +805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="185.25">
+    <row r="3" spans="1:7" ht="183.9">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -828,7 +828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="171">
+    <row r="4" spans="1:7" ht="169.75">
       <c r="A4" s="3" t="s">
         <v>19</v>
       </c>
@@ -851,7 +851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="199.5">
+    <row r="5" spans="1:7" ht="198">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -874,7 +874,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="185.25">
+    <row r="6" spans="1:7" ht="183.9">
       <c r="A6" s="3" t="s">
         <v>30</v>
       </c>
@@ -897,7 +897,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="142.5">
+    <row r="7" spans="1:7" ht="141.44999999999999">
       <c r="A7" s="3" t="s">
         <v>35</v>
       </c>
@@ -920,7 +920,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="142.5">
+    <row r="8" spans="1:7" ht="141.44999999999999">
       <c r="A8" s="3" t="s">
         <v>40</v>
       </c>
@@ -943,7 +943,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="99.75">
+    <row r="9" spans="1:7" ht="99">
       <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
@@ -966,7 +966,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="99.75">
+    <row r="10" spans="1:7" ht="99">
       <c r="A10" s="3" t="s">
         <v>51</v>
       </c>
@@ -989,7 +989,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="128.25">
+    <row r="11" spans="1:7" ht="127.3">
       <c r="A11" s="3" t="s">
         <v>56</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="128.25">
+    <row r="12" spans="1:7" ht="113.15">
       <c r="A12" s="3" t="s">
         <v>61</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="128.25">
+    <row r="13" spans="1:7" ht="127.3">
       <c r="A13" s="3" t="s">
         <v>66</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="99.75">
+    <row r="14" spans="1:7" ht="99">
       <c r="A14" s="3" t="s">
         <v>71</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="99.75">
+    <row r="15" spans="1:7" ht="99">
       <c r="A15" s="3" t="s">
         <v>76</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="99.75">
+    <row r="16" spans="1:7" ht="99">
       <c r="A16" s="3" t="s">
         <v>81</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="128.25">
+    <row r="17" spans="1:7" ht="127.3">
       <c r="A17" s="3" t="s">
         <v>86</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="71.25">
+    <row r="18" spans="1:7" ht="70.75">
       <c r="A18" s="3" t="s">
         <v>91</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="114">
+    <row r="19" spans="1:7" ht="99">
       <c r="A19" s="3" t="s">
         <v>96</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="128.25">
+    <row r="20" spans="1:7" ht="127.3">
       <c r="A20" s="3" t="s">
         <v>101</v>
       </c>

</xml_diff>